<commit_message>
feat: replace dates on every month on every date on schedule document
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -745,15 +745,13 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="B:AF"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="2" style="2" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="2" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="2" style="2" width="4.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="33" style="1" width="11.43"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat: fill schedule template for every ambient x every day
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="272">
   <si>
     <t xml:space="preserve">FORMATO / REGISTRO</t>
   </si>
@@ -61,97 +61,769 @@
     <t xml:space="preserve">{ambiente_1}</t>
   </si>
   <si>
-    <t xml:space="preserve">{a1}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a2}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a3}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a4}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a5}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a6}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a7}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a8}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a9}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a10}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a11}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a12}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a13}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a14}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a15}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a16}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a17}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a18}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a19}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a20}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a21}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a22}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a23}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a24}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a25}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a26}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a27}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a28}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a29}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a30}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a31}</t>
+    <t xml:space="preserve">{1_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{1_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{3_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{5_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{6_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{7_31}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ambiente_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_21}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_22}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_23}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_24}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_26}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_27}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_28}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_29}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{8_31}</t>
   </si>
   <si>
     <t xml:space="preserve">D=DESINSECTACIÓN,DESINFECCIONY DESRATIZACIÓN                                                    </t>
@@ -744,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF1" activeCellId="0" sqref="B:AF"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1182,247 +1854,695 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
+      <c r="A11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF11" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
+      <c r="A12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="T12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="U12" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="V12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="W12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="X12" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y12" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z12" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA12" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB12" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC12" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD12" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF12" s="14" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
+      <c r="A13" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="T13" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="U13" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="X13" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y13" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB13" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC13" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE13" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF13" s="14" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="14"/>
+      <c r="A14" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="R14" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="U14" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="X14" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA14" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB14" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD14" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE14" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF14" s="14" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
+      <c r="A15" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="T15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="X15" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y15" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z15" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA15" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB15" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC15" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD15" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="AE15" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF15" s="14" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="14"/>
+      <c r="A16" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="S16" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T16" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="U16" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="V16" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="X16" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y16" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z16" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA16" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB16" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC16" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD16" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE16" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF16" s="14" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
+    <row r="17" customFormat="false" ht="16.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="R17" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="V17" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="X17" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z17" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA17" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB17" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC17" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD17" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE17" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="AF17" s="14" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="17"/>
       <c r="B18" s="18" t="s">
-        <v>44</v>
+        <v>268</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -1520,7 +2640,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N22" s="26" t="s">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
@@ -1559,7 +2679,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="N25" s="27" t="s">
-        <v>46</v>
+        <v>270</v>
       </c>
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
@@ -1578,7 +2698,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="N26" s="26" t="s">
-        <v>47</v>
+        <v>271</v>
       </c>
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>

</xml_diff>

<commit_message>
feat: generate schedule excel
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -826,7 +826,7 @@
     <t xml:space="preserve">{8_31}</t>
   </si>
   <si>
-    <t xml:space="preserve">D=DESINSECTACIÓN,DESINFECCIONY DESRATIZACIÓN                                                    </t>
+    <t xml:space="preserve">D=DESINSECTACIÓN, I=DESINFECCION, R=DESRATIZACIÓN, F=FUMIGACIÓN, T=LIMPIEZA DE TANQUE</t>
   </si>
   <si>
     <t xml:space="preserve">ATENTAMENTE</t>
@@ -846,7 +846,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,6 +906,21 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="GeoSlab703 MdCn BT"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="GeoSlab703 MdCn BT"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="GeoSlab703 MdCn BT"/>
@@ -915,13 +930,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="GeoSlab703 MdCn BT"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="GeoSlab703 MdCn BT"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1086,27 +1094,27 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1114,11 +1122,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1417,7 +1425,7 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2539,7 +2547,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="17"/>
       <c r="B18" s="18" t="s">
         <v>268</v>
@@ -2554,45 +2562,48 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
-      <c r="M18" s="19"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21"/>
-      <c r="AE18" s="21"/>
-      <c r="AF18" s="21"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="19"/>
-      <c r="Q19" s="20"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="22"/>
+      <c r="Q19" s="23"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
       <c r="X19" s="24"/>
       <c r="Y19" s="24"/>
       <c r="Z19" s="24"/>
@@ -2604,26 +2615,26 @@
       <c r="AF19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="19"/>
-      <c r="Q20" s="20"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="22"/>
+      <c r="Q20" s="23"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
       <c r="Z20" s="24"/>
@@ -2636,7 +2647,7 @@
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25"/>
-      <c r="R21" s="20"/>
+      <c r="R21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N22" s="26" t="s">
@@ -2651,24 +2662,24 @@
       <c r="U22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="20"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="1"/>
@@ -2709,14 +2720,14 @@
       <c r="U26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="20"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2729,7 +2740,7 @@
     <mergeCell ref="B5:AF5"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="B7:AF7"/>
-    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B18:W18"/>
     <mergeCell ref="X18:AF18"/>
     <mergeCell ref="N22:U22"/>
     <mergeCell ref="N25:U25"/>

</xml_diff>

<commit_message>
fix: schedule document generation layout
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -955,7 +955,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -975,13 +975,6 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1022,111 +1015,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1213,9 +1206,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1220040</xdr:colOff>
+      <xdr:colOff>1219680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:rowOff>215640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1229,7 +1222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="521640" y="68760"/>
-          <a:ext cx="698400" cy="587880"/>
+          <a:ext cx="698040" cy="587520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1425,10 +1418,10 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="2" style="2" width="4.14"/>

</xml_diff>

<commit_message>
feat: add labels per combination to schedule
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -826,7 +826,7 @@
     <t xml:space="preserve">{8_31}</t>
   </si>
   <si>
-    <t xml:space="preserve">D=DESINSECTACIÓN, I=DESINFECCION, R=DESRATIZACIÓN, F=FUMIGACIÓN, T=LIMPIEZA DE TANQUE</t>
+    <t xml:space="preserve">{service_labels}</t>
   </si>
   <si>
     <t xml:space="preserve">ATENTAMENTE</t>
@@ -1206,9 +1206,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1277640</xdr:colOff>
+      <xdr:colOff>1276920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>214920</xdr:rowOff>
+      <xdr:rowOff>214200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1228,7 +1228,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="489960" y="11880"/>
-          <a:ext cx="787680" cy="643680"/>
+          <a:ext cx="786960" cy="642960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1424,10 +1424,10 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="2" style="2" width="4.14"/>

</xml_diff>

<commit_message>
feat: update logo in documents
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cronograma_plantilla.xlsx
+++ b/backend/src/Templates/cronograma_plantilla.xlsx
@@ -1197,22 +1197,22 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>489960</xdr:colOff>
+      <xdr:colOff>415800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1276920</xdr:colOff>
+      <xdr:colOff>1215360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>214200</xdr:rowOff>
+      <xdr:rowOff>212760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1227,8 +1227,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="489960" y="11880"/>
-          <a:ext cx="786960" cy="642960"/>
+          <a:off x="415800" y="0"/>
+          <a:ext cx="799560" cy="653400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1423,11 +1423,11 @@
   </sheetPr>
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="2" style="2" width="4.14"/>

</xml_diff>